<commit_message>
Fixed test data issue
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C4BA81-B522-4121-A9AC-B8DD81099B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6988A7-52C5-430D-B785-D88A909498CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XAlphaLogin" sheetId="9" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>PortfolioNumber</t>
   </si>
   <si>
-    <t>QA_TestCase_Auto_X-Alpha_004</t>
-  </si>
-  <si>
     <t>BTC</t>
   </si>
   <si>
@@ -117,19 +114,22 @@
     <t>FX Spot</t>
   </si>
   <si>
-    <t>QA_TestCase_Auto_X-Alpha_005</t>
-  </si>
-  <si>
     <t>buy</t>
   </si>
   <si>
     <t>pending</t>
   </si>
   <si>
-    <t>QA_TestCase_Auto_X-Alpha_006</t>
-  </si>
-  <si>
     <t>processed</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_XAlpha_004</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_XAlpha_005</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_XAlpha_006</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -182,17 +182,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,14 +552,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD5F807-ACA8-48C4-B9BD-3C44953A349F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.1796875" customWidth="1"/>
     <col min="4" max="4" width="21.26953125" customWidth="1"/>
     <col min="5" max="5" width="18.453125" customWidth="1"/>
@@ -588,6 +606,7 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="1" t="b">
         <v>0</v>
       </c>
@@ -608,6 +627,7 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="1" t="b">
         <v>0</v>
       </c>
@@ -628,6 +648,7 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
@@ -647,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -706,19 +727,19 @@
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -730,13 +751,13 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2">
         <v>8000</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2" s="1" t="b">
         <v>0</v>
@@ -744,19 +765,19 @@
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -768,13 +789,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3">
         <v>8000</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1" t="b">
         <v>0</v>
@@ -782,19 +803,19 @@
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -806,13 +827,13 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <v>8000</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N4" s="1" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Merged QA_TestCase_Auto_XAlpha_016 and QA_TestCase_Auto_XAlpha_017
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5CCD7E-17A2-4B4F-A501-053512AD3681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E50626-CD49-4977-A64D-A360D66AC958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -696,7 +696,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added deal type filter methods
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED68CD51-3E27-4861-A93E-99992BC97F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240BF73C-82C7-4AD8-9B50-6C0A6DAFCA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="2720" windowWidth="14400" windowHeight="7360" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XAlphaLogin" sheetId="9" r:id="rId1"/>
@@ -741,9 +741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Minor updates in XAlphaDealEnquiry tag
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CC0D27-6FB6-4882-8ADA-605C37A1A127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51549212-F65A-42F3-9B45-7E52BCF887DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -764,7 +764,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L19" sqref="L19"/>
+      <selection pane="topRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -778,6 +778,7 @@
     <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.453125" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -858,6 +859,9 @@
       <c r="K2" t="s">
         <v>29</v>
       </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
       <c r="N2" s="1" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Created locator and helper actions to update deal details
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B134E260-4A55-42BA-BE6D-AE23F635819B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055A980F-BE78-446E-A2C9-88130CF54719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="71">
   <si>
     <t>URL</t>
   </si>
@@ -199,13 +199,43 @@
   </si>
   <si>
     <t>cancelled</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_XAlpha_034</t>
+  </si>
+  <si>
+    <t>BaseAssetAmount_updated</t>
+  </si>
+  <si>
+    <t>Direction_updated</t>
+  </si>
+  <si>
+    <t>BaseAsset_updated</t>
+  </si>
+  <si>
+    <t>QuoteAsset_updated</t>
+  </si>
+  <si>
+    <t>UnitPrice_updated</t>
+  </si>
+  <si>
+    <t>FeeAsset_updated</t>
+  </si>
+  <si>
+    <t>FeeAmount_updated</t>
+  </si>
+  <si>
+    <t>CounterpartyName_updated</t>
+  </si>
+  <si>
+    <t>PortfolioNumber_updated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,16 +249,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -266,11 +322,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -281,6 +355,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,840 +856,2160 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:X1048565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.453125" customWidth="1"/>
-    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="10"/>
+    <col min="3" max="3" width="8.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.90625" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17" style="11" customWidth="1"/>
+    <col min="23" max="23" width="8.7265625" style="11"/>
+    <col min="24" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Q1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="S1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="U1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="V1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="W1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="7">
+        <v>1</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J2">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="7">
         <v>8000</v>
       </c>
-      <c r="K2" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M2">
-        <v>4</v>
-      </c>
-      <c r="N2" s="1" t="b">
+      <c r="U2" s="9"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H3" s="9"/>
+      <c r="I3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="7">
+        <v>1</v>
+      </c>
+      <c r="O3" s="9"/>
+      <c r="P3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J3">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="7">
         <v>8000</v>
       </c>
-      <c r="K3" t="s">
+      <c r="S3" s="9"/>
+      <c r="T3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="1" t="b">
+      <c r="U3" s="9"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="7">
+        <v>1</v>
+      </c>
+      <c r="O4" s="9"/>
+      <c r="P4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J4">
+      <c r="Q4" s="9"/>
+      <c r="R4" s="7">
         <v>8000</v>
       </c>
-      <c r="K4" t="s">
+      <c r="S4" s="9"/>
+      <c r="T4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="1" t="b">
+      <c r="U4" s="9"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+    <row r="5" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="7">
+        <v>1</v>
+      </c>
+      <c r="O5" s="9"/>
+      <c r="P5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J5">
+      <c r="Q5" s="9"/>
+      <c r="R5" s="7">
         <v>8000</v>
       </c>
-      <c r="K5" t="s">
+      <c r="S5" s="9"/>
+      <c r="T5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="1" t="b">
+      <c r="U5" s="9"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+    <row r="6" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="H6" s="9"/>
+      <c r="I6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="7">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9"/>
+      <c r="P6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J6">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7">
         <v>8000</v>
       </c>
-      <c r="K6" t="s">
+      <c r="S6" s="9"/>
+      <c r="T6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="1" t="b">
+      <c r="U6" s="9"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+    <row r="7" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="7">
+        <v>1</v>
+      </c>
+      <c r="O7" s="9"/>
+      <c r="P7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J7">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="7">
         <v>8000</v>
       </c>
-      <c r="K7" t="s">
+      <c r="S7" s="9"/>
+      <c r="T7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L7" t="s">
+      <c r="U7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="1" t="b">
+      <c r="V7" s="7"/>
+      <c r="W7" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+    <row r="8" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="7">
+        <v>1</v>
+      </c>
+      <c r="O8" s="9"/>
+      <c r="P8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J8">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="7">
         <v>8000</v>
       </c>
-      <c r="K8" t="s">
+      <c r="S8" s="9"/>
+      <c r="T8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L8" t="s">
+      <c r="U8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N8" s="1" t="b">
+      <c r="V8" s="7"/>
+      <c r="W8" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+    <row r="9" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="7">
+        <v>1</v>
+      </c>
+      <c r="O9" s="9"/>
+      <c r="P9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J9">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="7">
         <v>8000</v>
       </c>
-      <c r="K9" t="s">
+      <c r="S9" s="9"/>
+      <c r="T9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L9" t="s">
+      <c r="U9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="1" t="b">
+      <c r="V9" s="7"/>
+      <c r="W9" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+    <row r="10" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="7">
+        <v>1</v>
+      </c>
+      <c r="O10" s="9"/>
+      <c r="P10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J10">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="7">
         <v>8000</v>
       </c>
-      <c r="K10" t="s">
+      <c r="S10" s="9"/>
+      <c r="T10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="L10" t="s">
+      <c r="U10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="1" t="b">
+      <c r="V10" s="7"/>
+      <c r="W10" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+    <row r="11" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="7">
+        <v>1</v>
+      </c>
+      <c r="O11" s="9"/>
+      <c r="P11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J11">
+      <c r="Q11" s="9"/>
+      <c r="R11" s="7">
         <v>8000</v>
       </c>
-      <c r="K11" t="s">
+      <c r="S11" s="9"/>
+      <c r="T11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L11" t="s">
+      <c r="U11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="1" t="b">
+      <c r="V11" s="7"/>
+      <c r="W11" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+    <row r="12" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="H12" s="9"/>
+      <c r="I12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="7">
+        <v>1</v>
+      </c>
+      <c r="O12" s="9"/>
+      <c r="P12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J12">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="7">
         <v>8000</v>
       </c>
-      <c r="K12" t="s">
+      <c r="S12" s="9"/>
+      <c r="T12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L12" t="s">
+      <c r="U12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N12" s="1" t="b">
+      <c r="V12" s="7"/>
+      <c r="W12" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+    <row r="13" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="7">
+        <v>1</v>
+      </c>
+      <c r="O13" s="9"/>
+      <c r="P13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J13">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="7">
         <v>8000</v>
       </c>
-      <c r="K13" t="s">
+      <c r="S13" s="9"/>
+      <c r="T13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L13" t="s">
+      <c r="U13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N13" s="1" t="b">
+      <c r="V13" s="7"/>
+      <c r="W13" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+    <row r="14" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H14" s="9"/>
+      <c r="I14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="7">
+        <v>1</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="P14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J14">
+      <c r="Q14" s="9"/>
+      <c r="R14" s="7">
         <v>8000</v>
       </c>
-      <c r="K14" t="s">
+      <c r="S14" s="9"/>
+      <c r="T14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="L14" t="s">
+      <c r="U14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="1" t="b">
+      <c r="V14" s="7"/>
+      <c r="W14" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+    <row r="15" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="H15" s="9"/>
+      <c r="I15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="7">
+        <v>1</v>
+      </c>
+      <c r="O15" s="9"/>
+      <c r="P15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J15">
+      <c r="Q15" s="9"/>
+      <c r="R15" s="7">
         <v>8000</v>
       </c>
-      <c r="K15" t="s">
+      <c r="S15" s="9"/>
+      <c r="T15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L15" t="s">
+      <c r="U15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="1" t="b">
+      <c r="V15" s="7"/>
+      <c r="W15" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+    <row r="16" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="H16" s="9"/>
+      <c r="I16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="7">
+        <v>1</v>
+      </c>
+      <c r="O16" s="9"/>
+      <c r="P16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J16">
+      <c r="Q16" s="9"/>
+      <c r="R16" s="7">
         <v>8000</v>
       </c>
-      <c r="K16" t="s">
+      <c r="S16" s="9"/>
+      <c r="T16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L16" t="s">
+      <c r="U16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="1" t="b">
+      <c r="V16" s="7"/>
+      <c r="W16" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+    <row r="17" spans="1:24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="H17" s="9"/>
+      <c r="I17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="9"/>
+      <c r="N17" s="7">
+        <v>1</v>
+      </c>
+      <c r="O17" s="9"/>
+      <c r="P17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J17">
+      <c r="Q17" s="9"/>
+      <c r="R17" s="7">
         <v>8000</v>
       </c>
-      <c r="K17" t="s">
+      <c r="S17" s="9"/>
+      <c r="T17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L17" t="s">
+      <c r="U17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="1" t="b">
+      <c r="V17" s="7"/>
+      <c r="W17" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+    <row r="18" spans="1:24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="7">
+        <v>1</v>
+      </c>
+      <c r="O18" s="9"/>
+      <c r="P18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J18">
+      <c r="Q18" s="9"/>
+      <c r="R18" s="7">
         <v>8000</v>
       </c>
-      <c r="K18" t="s">
+      <c r="S18" s="9"/>
+      <c r="T18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="L18" t="s">
+      <c r="U18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="1" t="b">
+      <c r="V18" s="7"/>
+      <c r="W18" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+    <row r="19" spans="1:24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="H19" s="9"/>
+      <c r="I19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="7">
+        <v>1</v>
+      </c>
+      <c r="O19" s="9"/>
+      <c r="P19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J19">
+      <c r="Q19" s="9"/>
+      <c r="R19" s="7">
         <v>8000</v>
       </c>
-      <c r="K19" t="s">
+      <c r="S19" s="9"/>
+      <c r="T19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L19" t="s">
+      <c r="U19" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="N19" s="1" t="b">
+      <c r="V19" s="7"/>
+      <c r="W19" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+    <row r="20" spans="1:24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="H20" s="9"/>
+      <c r="I20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="7">
+        <v>1</v>
+      </c>
+      <c r="O20" s="9"/>
+      <c r="P20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J20">
+      <c r="Q20" s="9"/>
+      <c r="R20" s="7">
         <v>8000</v>
       </c>
-      <c r="K20" t="s">
+      <c r="S20" s="9"/>
+      <c r="T20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L20" t="s">
+      <c r="U20" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="N20" s="1" t="b">
+      <c r="V20" s="7"/>
+      <c r="W20" s="3" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="21" spans="1:24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="7">
+        <v>1</v>
+      </c>
+      <c r="O21" s="9"/>
+      <c r="P21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="7">
+        <v>8000</v>
+      </c>
+      <c r="S21" s="9"/>
+      <c r="T21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="U21" s="9"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+    </row>
+    <row r="23" spans="1:24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+    </row>
+    <row r="24" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+    </row>
+    <row r="33" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="34" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="35" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="36" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="37" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="38" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="39" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="40" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="41" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="42" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="43" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="44" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="45" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="47" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="48" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="49" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="50" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="53" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="54" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="55" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="56" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="57" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="58" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="59" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="60" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="61" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="62" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="63" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="64" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="65" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="66" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="67" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="68" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="69" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="70" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="71" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="72" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="73" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="74" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="75" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="76" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="77" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="78" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="79" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="80" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="81" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="82" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="83" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="84" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="85" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="86" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="87" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="88" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="89" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="90" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="91" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="92" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="93" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="94" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="95" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="96" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="97" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="98" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="99" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="100" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="101" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="102" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="103" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="104" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="105" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="106" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="107" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="108" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="109" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="110" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="111" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="112" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="113" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="114" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="115" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="116" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="117" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="118" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="119" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="120" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="121" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="122" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="123" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="124" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="125" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="126" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="127" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="128" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="129" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="130" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="131" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="132" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="133" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="134" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="135" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="136" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="137" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="138" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="139" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="140" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="141" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="142" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="143" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="144" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="145" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="146" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="147" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="148" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="149" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="150" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="151" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="152" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="153" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="154" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="155" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="156" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="157" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="158" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="159" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="160" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="161" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="162" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="163" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="164" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="165" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="166" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="167" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="168" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="169" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="170" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="171" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="172" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="173" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="174" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="175" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="176" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="177" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="178" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="179" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="180" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="181" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="182" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="183" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="184" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="185" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="186" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="187" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="188" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="189" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="190" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="191" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="192" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="193" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="194" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="195" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="196" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="197" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="198" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="199" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="200" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="201" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="202" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="203" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="204" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="205" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="206" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="207" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="208" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="209" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="210" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="211" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="212" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="213" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="214" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="215" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="216" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="217" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="218" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="219" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="220" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="221" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="222" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="223" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="224" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="225" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="226" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="227" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="228" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="229" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="230" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="231" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="232" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="233" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="234" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="235" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="236" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="237" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="238" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="239" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="240" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="241" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="242" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="243" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="244" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="245" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="246" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="247" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="248" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="249" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="250" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="251" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="252" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="253" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="254" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="255" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="256" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="257" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="258" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="259" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="260" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="261" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="262" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="263" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="264" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="265" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="266" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="267" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="268" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="269" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="270" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="271" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="272" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="273" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="274" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="275" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="276" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="277" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="278" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="279" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="280" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="281" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="282" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="283" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="284" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="285" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="286" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="287" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="288" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="289" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="290" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="291" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="292" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="293" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="294" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="295" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="296" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="297" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="298" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="299" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="300" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="301" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="302" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="303" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="304" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="305" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="306" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="307" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="308" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="309" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="310" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="311" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="312" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="313" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="314" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="315" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="316" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="317" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="318" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="319" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="320" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="321" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="322" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="323" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="324" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="325" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="326" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="327" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="328" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="329" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="330" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="331" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="332" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="333" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="334" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="335" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="336" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="337" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="338" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="339" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="340" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="341" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="342" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="343" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="344" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="345" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="346" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="347" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="348" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="349" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="350" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="351" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="352" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="353" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="354" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="355" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="356" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="357" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="358" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="359" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="360" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="361" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="362" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="363" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="364" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="365" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="366" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="367" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="368" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="369" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="370" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="371" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="372" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="373" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="374" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="375" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="376" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="377" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="378" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="379" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="380" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="381" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="382" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="383" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="384" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="385" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="386" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="387" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="388" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="389" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="390" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="391" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="392" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="393" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="394" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="395" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="396" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="397" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="398" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="399" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="400" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="401" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="402" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="403" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="404" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="405" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="406" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="407" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="408" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="409" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="410" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="411" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="412" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="413" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="414" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="415" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="416" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="417" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="418" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="419" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="420" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="421" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="422" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="423" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="424" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="425" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="426" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="427" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="428" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="429" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="430" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="431" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="432" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="433" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="434" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="435" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="436" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="437" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="438" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="439" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="440" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="441" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="442" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="443" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="444" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="445" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="446" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="447" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="448" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="449" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="450" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="451" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="452" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="453" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="454" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="455" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="456" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="457" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="458" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="459" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="460" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="461" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="462" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="463" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="464" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="465" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="466" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="467" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="468" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="469" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="470" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="471" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="472" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="473" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="474" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="475" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="476" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="477" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="478" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="479" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="480" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="481" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="482" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="483" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="484" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="485" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="486" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="487" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="488" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="489" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="490" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="491" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="492" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="493" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="494" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="495" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="496" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="497" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="498" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="499" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="500" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="501" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="502" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="503" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="504" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="505" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="506" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="507" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="508" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="509" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="510" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="511" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="512" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="513" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="514" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="515" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="516" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="517" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="518" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="519" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="520" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="521" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="522" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="523" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="524" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="525" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="526" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="527" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="528" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="529" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="530" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="531" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="532" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="533" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="534" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="535" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="536" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="537" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="538" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="539" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="540" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="541" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="542" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="543" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="544" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="545" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="546" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="547" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="548" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="549" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="550" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="551" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="552" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="553" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="554" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="555" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="556" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="557" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="558" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="559" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="560" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="561" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="562" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="563" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="564" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="565" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="566" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="567" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="568" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="569" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="570" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="571" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="572" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="573" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="574" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="575" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="576" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="577" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="578" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="579" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="580" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="581" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="582" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="583" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="584" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="585" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="586" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="587" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="588" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="589" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="590" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="591" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="592" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="593" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="594" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="595" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="596" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="597" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="598" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="599" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="600" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="601" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="602" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="603" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="604" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="605" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="606" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="607" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="608" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="609" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="610" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="611" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="612" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="613" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="614" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="615" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="616" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="617" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="618" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="619" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="620" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="621" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="622" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="623" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="624" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="625" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="626" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="627" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="628" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="629" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="630" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="631" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="632" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="633" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="634" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="635" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="636" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="637" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="638" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="639" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="640" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="641" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="642" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="643" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="644" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="645" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="646" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="647" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="648" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="649" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="650" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="651" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="652" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="653" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="654" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="655" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="656" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="657" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="658" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="659" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="660" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="661" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="662" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="663" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="664" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="665" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="666" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="667" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="668" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="669" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="670" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="671" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="672" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="673" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="674" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="675" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="676" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="677" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="678" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="679" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="680" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="681" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="682" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="683" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="684" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="685" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="686" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="687" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="688" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="689" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="690" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="691" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="692" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="693" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="694" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="695" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="696" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="697" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="698" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="699" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="700" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="701" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="702" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="703" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="704" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="705" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="706" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="707" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="708" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="709" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="710" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="711" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="712" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="713" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="714" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="715" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="716" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="717" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="718" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="719" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="720" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="721" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="722" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="723" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="724" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="725" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="726" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="727" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="728" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="729" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="730" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="731" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="732" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="733" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="734" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="735" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="736" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="737" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="738" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="739" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="740" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="741" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="742" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="743" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="744" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="745" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="746" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="747" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="748" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="749" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="750" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="751" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="752" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="753" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="754" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="755" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="756" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="757" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="758" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="759" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="760" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="761" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="762" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="763" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="764" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="765" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="766" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="767" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="768" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="769" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="770" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="771" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="772" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="773" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="774" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="775" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="776" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="777" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="778" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="779" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="780" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="781" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="782" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="783" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="784" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="785" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="786" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="787" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="788" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="789" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="790" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="791" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="792" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="793" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="794" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="795" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="796" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="797" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="798" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="799" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="800" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="1048562" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D1048562" s="14"/>
+    </row>
+    <row r="1048565" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D1048565" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added system.qa.checker user into test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A29058F-70F7-4941-AFA8-F8395785E051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA30F77-901B-4E27-9E66-62E0A07F35D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="92">
   <si>
     <t>Username</t>
   </si>
@@ -142,9 +142,6 @@
     <t>QA_TestCase_Auto_XAlpha_016</t>
   </si>
   <si>
-    <t>alen.key</t>
-  </si>
-  <si>
     <t>QA_TestCase_Auto_XAlpha_017</t>
   </si>
   <si>
@@ -287,6 +284,15 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_XAlpha_044</t>
+  </si>
+  <si>
+    <t>system.qa.checker</t>
+  </si>
+  <si>
+    <t>J6cxU20ke24l</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_XAlpha_045</t>
   </si>
 </sst>
 </file>
@@ -784,7 +790,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -873,7 +879,7 @@
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -891,13 +897,13 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="1" t="b">
@@ -963,52 +969,52 @@
         <v>15</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>22</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>21</v>
@@ -1039,16 +1045,16 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="7">
@@ -1056,7 +1062,7 @@
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q2" s="9"/>
       <c r="R2" s="7">
@@ -1088,16 +1094,16 @@
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="7">
@@ -1105,7 +1111,7 @@
       </c>
       <c r="O3" s="9"/>
       <c r="P3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="9"/>
       <c r="R3" s="7">
@@ -1137,16 +1143,16 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="7">
@@ -1154,7 +1160,7 @@
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" s="7">
@@ -1186,16 +1192,16 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="7">
@@ -1203,7 +1209,7 @@
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="7">
@@ -1235,16 +1241,16 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="7">
@@ -1252,7 +1258,7 @@
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="7">
@@ -1270,7 +1276,7 @@
     </row>
     <row r="7" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>26</v>
@@ -1284,16 +1290,16 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="7">
@@ -1301,7 +1307,7 @@
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q7" s="9"/>
       <c r="R7" s="7">
@@ -1333,16 +1339,16 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="7">
@@ -1350,7 +1356,7 @@
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="7">
@@ -1384,16 +1390,16 @@
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="7">
@@ -1401,7 +1407,7 @@
       </c>
       <c r="O9" s="9"/>
       <c r="P9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q9" s="9"/>
       <c r="R9" s="7">
@@ -1435,16 +1441,16 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M10" s="9"/>
       <c r="N10" s="7">
@@ -1452,7 +1458,7 @@
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q10" s="9"/>
       <c r="R10" s="7">
@@ -1472,7 +1478,7 @@
     </row>
     <row r="11" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>26</v>
@@ -1486,16 +1492,16 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="7">
@@ -1503,7 +1509,7 @@
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q11" s="9"/>
       <c r="R11" s="7">
@@ -1523,7 +1529,7 @@
     </row>
     <row r="12" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>26</v>
@@ -1537,16 +1543,16 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M12" s="9"/>
       <c r="N12" s="7">
@@ -1554,7 +1560,7 @@
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q12" s="9"/>
       <c r="R12" s="7">
@@ -1574,7 +1580,7 @@
     </row>
     <row r="13" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>26</v>
@@ -1588,16 +1594,16 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" s="7">
@@ -1605,7 +1611,7 @@
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q13" s="9"/>
       <c r="R13" s="7">
@@ -1625,7 +1631,7 @@
     </row>
     <row r="14" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>26</v>
@@ -1639,16 +1645,16 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="7">
@@ -1656,7 +1662,7 @@
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q14" s="9"/>
       <c r="R14" s="7">
@@ -1676,7 +1682,7 @@
     </row>
     <row r="15" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>26</v>
@@ -1690,16 +1696,16 @@
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="7">
@@ -1707,7 +1713,7 @@
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q15" s="9"/>
       <c r="R15" s="7">
@@ -1727,7 +1733,7 @@
     </row>
     <row r="16" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>26</v>
@@ -1741,16 +1747,16 @@
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M16" s="9"/>
       <c r="N16" s="7">
@@ -1758,7 +1764,7 @@
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q16" s="9"/>
       <c r="R16" s="7">
@@ -1778,7 +1784,7 @@
     </row>
     <row r="17" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>26</v>
@@ -1792,16 +1798,16 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="7">
@@ -1809,7 +1815,7 @@
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q17" s="9"/>
       <c r="R17" s="7">
@@ -1829,7 +1835,7 @@
     </row>
     <row r="18" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>26</v>
@@ -1843,16 +1849,16 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M18" s="9"/>
       <c r="N18" s="7">
@@ -1860,7 +1866,7 @@
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q18" s="9"/>
       <c r="R18" s="7">
@@ -1880,7 +1886,7 @@
     </row>
     <row r="19" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>26</v>
@@ -1894,16 +1900,16 @@
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="7">
@@ -1911,7 +1917,7 @@
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q19" s="9"/>
       <c r="R19" s="7">
@@ -1931,7 +1937,7 @@
     </row>
     <row r="20" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>26</v>
@@ -1945,16 +1951,16 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="7">
@@ -1962,7 +1968,7 @@
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q20" s="9"/>
       <c r="R20" s="7">
@@ -1973,7 +1979,7 @@
         <v>24</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V20" s="7"/>
       <c r="W20" s="3" t="b">
@@ -1982,7 +1988,7 @@
     </row>
     <row r="21" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>26</v>
@@ -1996,16 +2002,16 @@
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="7">
@@ -2013,7 +2019,7 @@
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q21" s="9"/>
       <c r="R21" s="7">
@@ -2024,7 +2030,7 @@
         <v>28</v>
       </c>
       <c r="U21" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V21" s="7"/>
       <c r="W21" s="3" t="b">
@@ -2033,7 +2039,7 @@
     </row>
     <row r="22" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>26</v>
@@ -2047,16 +2053,16 @@
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="7">
@@ -2064,7 +2070,7 @@
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q22" s="9"/>
       <c r="R22" s="7">
@@ -2075,7 +2081,7 @@
         <v>29</v>
       </c>
       <c r="U22" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V22" s="7"/>
       <c r="W22" s="3" t="b">
@@ -2084,7 +2090,7 @@
     </row>
     <row r="23" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>26</v>
@@ -2098,16 +2104,16 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="7">
@@ -2115,7 +2121,7 @@
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q23" s="9"/>
       <c r="R23" s="7">
@@ -2126,7 +2132,7 @@
         <v>34</v>
       </c>
       <c r="U23" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V23" s="7"/>
       <c r="W23" s="3" t="b">
@@ -2135,7 +2141,7 @@
     </row>
     <row r="24" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>26</v>
@@ -2153,25 +2159,25 @@
         <v>2</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H24" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="K24" s="9">
         <v>31638.25</v>
       </c>
       <c r="L24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="N24" s="7">
         <v>1</v>
@@ -2180,10 +2186,10 @@
         <v>2</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R24" s="7">
         <v>8000</v>
@@ -2202,7 +2208,7 @@
     </row>
     <row r="25" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>26</v>
@@ -2220,25 +2226,25 @@
         <v>3</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H25" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="K25" s="9">
         <v>31700.25</v>
       </c>
       <c r="L25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M25" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="M25" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="N25" s="7">
         <v>1</v>
@@ -2247,10 +2253,10 @@
         <v>3</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R25" s="7">
         <v>8000</v>
@@ -2269,7 +2275,7 @@
     </row>
     <row r="26" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>26</v>
@@ -2287,25 +2293,25 @@
         <v>3</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H26" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="K26" s="9">
         <v>31700.25</v>
       </c>
       <c r="L26" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M26" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="N26" s="7">
         <v>1</v>
@@ -2314,10 +2320,10 @@
         <v>3</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R26" s="7">
         <v>8000</v>
@@ -2336,7 +2342,7 @@
     </row>
     <row r="27" spans="1:23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>26</v>
@@ -2354,25 +2360,25 @@
         <v>3</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H27" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="K27" s="9">
         <v>31700.25</v>
       </c>
       <c r="L27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M27" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="M27" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="N27" s="7">
         <v>1</v>
@@ -2381,10 +2387,10 @@
         <v>3</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R27" s="7">
         <v>8000</v>
@@ -3303,9 +3309,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AAE02B-1ED2-44CD-BC76-39A59421CF46}">
   <dimension ref="A1:Q773"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3336,31 +3342,31 @@
         <v>25</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>20</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>22</v>
@@ -3383,25 +3389,25 @@
     </row>
     <row r="2" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>78</v>
-      </c>
       <c r="C2" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="17">
         <v>1</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" s="17">
         <v>2000</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="17">
         <v>1</v>
@@ -3414,7 +3420,7 @@
       </c>
       <c r="K2" s="22"/>
       <c r="L2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M2" s="7">
         <v>8000</v>
@@ -3430,25 +3436,25 @@
     </row>
     <row r="3" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="17">
         <v>1</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="17">
         <v>2000</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="17">
         <v>1</v>
@@ -3461,7 +3467,7 @@
       </c>
       <c r="K3" s="22"/>
       <c r="L3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M3" s="7">
         <v>8000</v>
@@ -3477,10 +3483,10 @@
     </row>
     <row r="4" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -3491,7 +3497,7 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -3508,10 +3514,10 @@
     </row>
     <row r="5" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -3522,7 +3528,7 @@
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
       <c r="K5" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -3537,23 +3543,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
+    <row r="6" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>

</xml_diff>

<commit_message>
Updated Provide FX Spot deal input details step definition
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68748F56-D773-4D4E-A048-0D81201C6CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD31062-9F01-4F8C-ACAB-1BBFE7018E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" tabRatio="644" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XAlphaLogin" sheetId="9" r:id="rId1"/>
@@ -1098,9 +1098,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:Y1048575"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P2" sqref="P2"/>
+      <selection pane="topRight" activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6548,7 +6548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21695F8F-FC0D-4216-9C70-4A42E90CA651}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed QA_TestCase_Auto_XAlpha_065 and value date issue on 4 other scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EE8FBB-A058-473C-AC5A-E0907D8D72D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA3E691-BA90-4E34-B0F5-CB696F6F0B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21367" yWindow="-100" windowWidth="21467" windowHeight="11443" tabRatio="644" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XAlphaLogin" sheetId="9" r:id="rId1"/>
@@ -4116,9 +4116,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AAE02B-1ED2-44CD-BC76-39A59421CF46}">
   <dimension ref="A1:AE780"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5615,19 +5615,19 @@
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K29" s="17"/>
       <c r="L29" s="9">
-        <v>2100</v>
+        <v>1900</v>
       </c>
       <c r="M29" s="17" t="s">
         <v>67</v>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="O29" s="17"/>
       <c r="P29" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="17"/>
       <c r="R29" s="9">
@@ -6557,7 +6557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21695F8F-FC0D-4216-9C70-4A42E90CA651}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed test case order of QA_TestCase_Auto_XAlpha_065
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA3E691-BA90-4E34-B0F5-CB696F6F0B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8CE752-4619-401F-B742-3AC03E74A95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21367" yWindow="-100" windowWidth="21467" windowHeight="11443" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XAlphaLogin" sheetId="9" r:id="rId1"/>
@@ -4116,9 +4116,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AAE02B-1ED2-44CD-BC76-39A59421CF46}">
   <dimension ref="A1:AE780"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomLeft" activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updates for failed Test Cases due to slowness or other issues
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/XAlpha.xlsx
+++ b/src/test/resources/testData/XAlpha.xlsx
@@ -6677,8 +6677,8 @@
   <dimension ref="A1:W812"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O36" sqref="O36"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7958,7 +7958,7 @@
       <c r="N25" s="25"/>
       <c r="O25" s="9"/>
       <c r="P25" s="7" t="s">
-        <v>173</v>
+        <v>28</v>
       </c>
       <c r="Q25" s="9" t="s">
         <v>54</v>

</xml_diff>